<commit_message>
Connect api, view movie using api, show list video using api
</commit_message>
<xml_diff>
--- a/server/src/movieUploader/movieList.xlsx
+++ b/server/src/movieUploader/movieList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sh4dy\Desktop\movieUploader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sh4dy\Desktop\movie\server\src\movieUploader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEDCE2A-E08E-4BFE-AF45-E695FED2FDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFB867-6058-4B3A-A7C9-AD5714B00FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17730" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{B5D7A5EF-DE06-4388-B4A5-FF8C956D4271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5D7A5EF-DE06-4388-B4A5-FF8C956D4271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="236">
   <si>
     <t>name</t>
   </si>
@@ -182,13 +182,571 @@
   </si>
   <si>
     <t>episode_url</t>
+  </si>
+  <si>
+    <t>12 Kỵ Binh Quả Cảm</t>
+  </si>
+  <si>
+    <t>Mỹ</t>
+  </si>
+  <si>
+    <t>Nhóm bộ binh 12 người được cử đến Afghanistan để tham gia trận đánh tiêu diệt Taliban và đồng minh AlQueda. Họ đã cùng kỵ binh Afghanistan thay đổi cục diện cuộc chiến.</t>
+  </si>
+  <si>
+    <t>Chris Hemsworth, Michael Shannon, Michael Pena</t>
+  </si>
+  <si>
+    <t>Phim hành động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/08/13/0as0xkb2_1920x1080-12kybinhquacam_296_168.webp                                                                                                                               </t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_12KyBinhQuaCam.mp4</t>
+  </si>
+  <si>
+    <t>HanhDong</t>
+  </si>
+  <si>
+    <t>13 tiếng</t>
+  </si>
+  <si>
+    <t>Một nhóm đặc vụ được giao trọng trách bảo vệ CIA phải vượt qua vô vàn thử thách khi khủng bố tấn công khu phức hợp ngoại giao ở Benghazi.</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/04/04/o20fe6xn_1920x1080-13tieng_296_168.webp</t>
+  </si>
+  <si>
+    <t>Gerard Butler, Lena Headey, David Wenham, Dominic West, Vincent Regan</t>
+  </si>
+  <si>
+    <t>Cuộc chiến của 300 chiến binh Spartan trước đạo quân Ba Tư đông đảo.</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/11/19/v91o79gp_1920x1080-300_296_168.webp</t>
+  </si>
+  <si>
+    <t>Thần đồng Hiro và robot Baymax là đôi bạn thân. Trong 1 lần có biến bị bọn xấu tấn công, Hiro và Baymax lập Biệt đội Big hero 6 truy tìm kẻ giấu mặt.</t>
+  </si>
+  <si>
+    <t>Biệt Đội Big Hero 6</t>
+  </si>
+  <si>
+    <t>Scott Adsit, Ryan Potter, Jamie Chung, Stan Lee, Daniel Henney, James Cromwell</t>
+  </si>
+  <si>
+    <t>Phim thiếu nhi</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_BigHero6_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/01/16/rdtgjsim_1920x1080_bighero602_296_168.webp</t>
+  </si>
+  <si>
+    <t>Biệt Đội Siêu Anh Hùng</t>
+  </si>
+  <si>
+    <t>Biệt đội siêu anh hùng với khả năng đặc biệt gồm: Người Sắt, Thần Sấm, Đội trưởng Mỹ, Người Khổng Lồ Xanh, Góa Phụ Đen cùng hợp lực cứu nguy thế giới.</t>
+  </si>
+  <si>
+    <t>Robert Downey Jr., Chris Evans, Tom Hiddleston, Chris Hemsworth, Jeremy Renner, Mark Ruffalo, Scarlett Johansson, Don Cheadle, Stan Lee, Gwyneth Paltrow, Samuel L. Jackson, Cobie Smulders</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_BietDoiSieuAnhHung1_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/28/4o9a6fsb_1920x1080-bietdoisieuanhhuyultron_296_168.webp</t>
+  </si>
+  <si>
+    <t>Annablle ra đời</t>
+  </si>
+  <si>
+    <t>Một nữ tu sĩ cùng các cô gái ở một trại trẻ mồ côi bị đóng cửa trở thành mục tiêu của một con búp bê bị quỷ ám.</t>
+  </si>
+  <si>
+    <t>Stephanie Sigman, Talitha Bateman, Anthony LaPaglia</t>
+  </si>
+  <si>
+    <t>Phim kinh dị</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_Annabelle_RaDoi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/04/12/yut18zn4_1920x1080-annabelleradoi_296_168.webp</t>
+  </si>
+  <si>
+    <t>Captain America 2 Chiến Binh Mùa Đông</t>
+  </si>
+  <si>
+    <t>​Trong vũ trụ Marvel, chiến binh mùa đông trong Captain America trở dậy hòa nhập cuộc sống mới đã cùng góa phụ áo đen đánh tan âm mưu phá thế giới.</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_CaptainAmerica_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>Chris Evans, Sebastian Stan, Scarlett Johansson, Elizabeth Olsen, Samuel L. Jackson, Cobie Smulders, Hayley Atwell, Emily VanCamp</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/28/beutcubx_1920x1080_chienbinhmuadong_296_168.webp</t>
+  </si>
+  <si>
+    <t>Câu Chuyện Đồ Chơi 3</t>
+  </si>
+  <si>
+    <t>​Để tránh bị quăng ra bãi rác sau khi cậu chủ Andy lên học Cao Đẳng, Buzz cùng nhóm bạn tìm cách lẻn vào thùng hàng đưa đến nhà trẻ Sunnyside mãi mãi.</t>
+  </si>
+  <si>
+    <t>Tom Hanks, Ned Beatty, Jeff Garlin, Don Rickles, Michael Keaton, Lee Unkrich</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/14/5brpaso2_1920x1080-cauchuyendochoi3_296_168.webp</t>
+  </si>
+  <si>
+    <t>Cướp Biển Vùng Caribbe 2 Chiếc Rương Thần Kỳ</t>
+  </si>
+  <si>
+    <t>​Cướp biển vùng Caribbean: Chiếc rương thần kỳ nói về việc thuyền trưởng Jack Sparrow phải trả món nợ với Davy Jones, truy tìm trái tim được cất giữ trong 1 chiếc rương của hắn</t>
+  </si>
+  <si>
+    <t>Johnny Depp, Orlando Bloom, Keira Knightley</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/22/45cw33z3_1920x1080cuopbiencaribechiecruongthanky_296_168.webp</t>
+  </si>
+  <si>
+    <t>Dạ Quỷ</t>
+  </si>
+  <si>
+    <t>Hyun Bin, Jang Dong Gun, Jo Woo Jin</t>
+  </si>
+  <si>
+    <t>Phim chiếu rạp</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_DaQuy.mp4</t>
+  </si>
+  <si>
+    <t>Hàn Quốc</t>
+  </si>
+  <si>
+    <t>Phiên bản cổ trang của "Chuyến tàu sinh tử". Hoàng tử Lee đau lòng khi chứng kiến cả giang sơn chìm trong đại dịch. Liệu vị hoàng tử có ngăn được cơn cuồng nộ của quỷ dữ?</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/22/yz4w5b1v_1920x1080-daquy_296_168.webp</t>
+  </si>
+  <si>
+    <t>Đại Chiến Thành Ansi</t>
+  </si>
+  <si>
+    <t>Một cuộc chiến không cân sức giữa 5 ngàn lính Goguryeo đối đầu với 20 vạn quân Đường để bảo vệ thành Ansi. Liệu đội Goguryeo có tạo nên kỳ tích?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo In Sung, Nam Joo Hyuk, Kim Seol Hyun, Yoo Oh Sung, </t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/08/13/4g3jww7i_1920x1080-daichienthanhansi_296_168.webp</t>
+  </si>
+  <si>
+    <t>Đại Chiến Titan Live Action Phần 1</t>
+  </si>
+  <si>
+    <t>Nhật Bản</t>
+  </si>
+  <si>
+    <t>Attack On Titan mang đến một cốt truyện bí ẩn, li kì, nhiều hành động và có yếu tố kinh dị. Đó là cuộc chiến của con người chống lại các Titan khổng lồ để giành giật mạng sống của mình.</t>
+  </si>
+  <si>
+    <t>Haruma Miura, Kiko Mizuhara, Hongo Kanata</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/08/16/8g5zsdfe_1920x1080-attackontitan-liveaction_296_168.webp</t>
+  </si>
+  <si>
+    <t>Đại Chiến Titan Live Action Phần 2</t>
+  </si>
+  <si>
+    <t>​Titan - 1 loài vật giống người, cực kì to lớn, nhưng óc như trái nho, thích ăn thịt người (Có thể coi đây là một dạng zombie). Còn con người thì hoàn toàn lép vế và phải cố thủ trong ba bức tường kiên cố, nhờ vậy mà họ đã có được 100 năm yên bình.</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/08/16/7swj2mt5_1920x1080-attackontitan-liveaction-2_296_168.webp</t>
+  </si>
+  <si>
+    <t>Điệp Vụ Tam Giác Vàng</t>
+  </si>
+  <si>
+    <t>Trung Quốc</t>
+  </si>
+  <si>
+    <t>Cuộc chiến chống lại tên trùm ma túy Naw Kham của chính phủ bốn nước Thái Lan, Lào, Myanmar và Trung Quốc tại khu vực Tam giác Vàng.</t>
+  </si>
+  <si>
+    <t>Trương Hàm Dư, Bành Vu Yến</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/01/04/ziwe1vyj_1920x1080-diepvutamgiacvang_296_168.webp</t>
+  </si>
+  <si>
+    <t>Gia Đình Siêu Nhân</t>
+  </si>
+  <si>
+    <t>Là một trong những phim hoạt hình về siêu nhân hay nhất, xoay quanh câu chuyện gia đình siêu anh hùng Parr.  Mỗi thành viên trong gia đình đều có sức mạnh đặc biệt.</t>
+  </si>
+  <si>
+    <t>Holly Hunter, Brad Bird, Wallace Shawn, Jason Lee, Craig T. Nelson, Samuel L. Jackson</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_GiaDinhSieuNhan_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/20/u9t9zmuz_1920x1080-giadinhsieunhan_296_168.webp</t>
+  </si>
+  <si>
+    <t>Giải Cứu Nhà Trắng</t>
+  </si>
+  <si>
+    <t>Cùng con gái nhỏ tham quan Nhà Trắng trong kỳ nghỉ cuối tuần. Ngờ đâu, Cale phải chiến đấu để cứu con gái và bảo vệ tổng thống khi nơi đó đang là mục tiêu khủng bố.</t>
+  </si>
+  <si>
+    <t>Channing Tatum, Jamie Foxx, Maggie Gyllenhaal, Jason Clarke, James Woods</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_GiaiCuuNhaTrang.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2020/12/28/zp7h25en_1920x1080giaicuunhatrang_296_168.webp</t>
+  </si>
+  <si>
+    <t>Harry Potter 1 Harry Potter Và Hòn Đá Phù Thủy</t>
+  </si>
+  <si>
+    <t>Harry Potter phát hiện ra cậu là phù thủy và được mời đến trường Hogwarts để học phép thuật. Nơi đây là thế giới hoàn toàn mới lạ với cậu. Cậu phải học cách thích nghi và cậu nhanh chóng nhận ra không phải mọi phù thủy đều đáng tin cậy.</t>
+  </si>
+  <si>
+    <t>Daniel Radcliffe, Rupert Grint, Emma Watson</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_HarryPotterAndTheSorcererStone.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/08/03/ytiijjqp_1920x1080-harrypotter-1_296_168.webp</t>
+  </si>
+  <si>
+    <t>Phim gia đình</t>
+  </si>
+  <si>
+    <t>Âu Mỹ</t>
+  </si>
+  <si>
+    <t>Harry Potter 2 Harry Potter Và Phòng Chứa Bí Mật</t>
+  </si>
+  <si>
+    <t>Câu chuyện xảy ra khi Harry bước vào năm thứ hai ở trường phép thuật. Trên tường của hành lang xuất hiện một loạt các tin nhắn, cảnh báo về việc phòng chứa bí mật đã được mở và người thừa kế của Slytherin sẽ sát hại những học sinh Máu bùn.</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_HARRYPOTTERANDTHECHAMBEROFSECRETS.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/08/03/wftdxtyf_1920x1080-harrypotter-2_296_168.webp</t>
+  </si>
+  <si>
+    <t>Khách Sạn Huyền Bí</t>
+  </si>
+  <si>
+    <t>Mang đến tiếng cười cùng nhiều bài học gia đình ý nghĩa, phim nhanh chóng chiếm được tình cảm của khán giả với câu chuyện về Bá tước Dracula "cute hạt me" cùng "bè lũ quái vật".</t>
+  </si>
+  <si>
+    <t>Adam Sandler, Kevin James, Andy Samberg</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_KhachSanHuyenBi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/07/07/trhkmmpo_1920x1080-khachsanhuyenbi1_296_168.webp</t>
+  </si>
+  <si>
+    <t>Kỷ Băng Hà 4 Lục Địa Trôi Dạt</t>
+  </si>
+  <si>
+    <t>​Kỷ băng hà 4 được đánh giá là loạt phim hoạt hình yêu thích và thành công nhất. Lần này bộ ba phải đối mặt với những thử thách do các lục địa bị trôi dạt sau trận đại hồng thủy</t>
+  </si>
+  <si>
+    <t>Ray Romano, Denis Leary, John Leguizamo, Nicki Minaj, Chris Wedge</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/20/wab9tpfg_1920x1080-kybangha4_296_168.webp</t>
+  </si>
+  <si>
+    <t>Lính Bắn Tỉa Mỹ</t>
+  </si>
+  <si>
+    <t>Câu chuyện về những trăn trở của Chris Kyle, người được mệnh danh là lính bắn tỉa giỏi nhất trong lịch sử quân đội Hoa Kì.</t>
+  </si>
+  <si>
+    <t>Bradley Cooper, Sienna Miller, Kyle Gallner</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_HBO_AmericanSniper_LinhBanTiaMy.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/04/07/5oe2umg3_1920x1080-linhbantiamy_296_168.webp</t>
+  </si>
+  <si>
+    <t>Long Ấn Cơ Mật</t>
+  </si>
+  <si>
+    <t>Phim là hành trình huyền bí trên lãnh thổ Trung Hoa để hoàn thành bản đồ Miền đông nước Nga của nhà thám hiểm Jonathan Green</t>
+  </si>
+  <si>
+    <t>Thành Long, Diêu Tinh Đồng, Jason Flemyng</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/02/16/yo42rncq_1920x1080-longancomat_296_168.webp</t>
+  </si>
+  <si>
+    <t>Người Hobbit 3 Đại Chiến 5 Cánh Quân</t>
+  </si>
+  <si>
+    <t>Sau khi thành công tiến vào lãnh địa của con rồng Smaug, anh chàng Hobbit gan dạ Bilbo cùng những người đồng đội Dwarf của mình sẽ phải đối mặt với những nguy hiểm gì? Những đội quân Orc đang rình rập, liệu Thor Oakenshield có thành công giành lại vương quốc của mình hay không, và số phận của vùng Trung Địa sẽ xoay chuyển như thế nào khi thế lực bóng tối từ Modor dần dần hiện thân.</t>
+  </si>
+  <si>
+    <t>Ian McKellen, Martin Freeman, Richard Armitage, Luke Evans, Lee Pace, Nghệ sĩ Orlando Bloom, Cate Blanchett, Cate Blanchett</t>
+  </si>
+  <si>
+    <t>Phim cổ trang</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_NguoiHobbit_DaiChienNamCanhQuan.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/11/04/r6o3jrek_1920x1080daichien5canhquan_296_168.webp</t>
+  </si>
+  <si>
+    <t>Người Nhện 6 Trở Về Nhà</t>
+  </si>
+  <si>
+    <t>Được chuyển thể từ truyện tranh cùng tên của Marvel, với kinh phí 175 triệu USD, đây là một trong những bộ phim siêu anh hùng hoành tráng nhất 2017.</t>
+  </si>
+  <si>
+    <t>Tom Holland, Michael Keaton, Robert Downey Jr.</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_NguoiNhen_TroVeNha.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/06/29/jfghmnm8_1920x1080-nguoinhentrovenha_296_168.webp</t>
+  </si>
+  <si>
+    <t>Người Vận Chuyển 2</t>
+  </si>
+  <si>
+    <t>​Chán với công việc người vận chuyển, Frank về Miami làm tài xế đưa đón cậu bé Jack của một gia đình giàu có. Jack bị bắt cóc, Frank đi cứu vô tình liên lụy vào tổ chức khủng bố</t>
+  </si>
+  <si>
+    <t>Jason Statham, Amber Valletta, Kate Nauta, Matthew Modine</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/28/fh2xiw44_1920x1080nguoivanchuyen2_296_168.webp</t>
+  </si>
+  <si>
+    <t>Nhà Trắng Thất Thủ Kẻ Phản Bội</t>
+  </si>
+  <si>
+    <t>Ám sát đương kim tổng thống Allan Trumbull, việc Mike Banning chưa bao giờ nghĩ tới đã khiến anh phải chạy trốn vì bị cáo buộc. Ai thực sự là kẻ phản bội khiến nhà trắng thất thủ?</t>
+  </si>
+  <si>
+    <t>Gerard Butler, Morgan Freeman, Danny Huston, Jada Pinkett Smith</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_AngelHasFallen1_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2022/03/15/wszc7994_1920x1080-nhatrangthatthukephanboi_296_168.webp</t>
+  </si>
+  <si>
+    <t>Quỷ Quyệt 2</t>
+  </si>
+  <si>
+    <t>Quỷ Quyệt 2 bắt đầu câu chuyện khi Josh đưa con trai trở về an toàn từ cõi âm nhưng lại bị một vong hồn khác ám vào thân xác khiến Josh phải chiến đấu để được quay về với gia đình</t>
+  </si>
+  <si>
+    <t>Patrick Wilson, Rose Byrne, Barbara Hershey</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/01.2021/0203/Teaser_QuyQuyet2.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2020/12/22/usofj521_1920x1080quyquyet2_296_168.webp</t>
+  </si>
+  <si>
+    <t>Sát Thủ John Wick 3 Chuẩn Bị Chiến Tranh</t>
+  </si>
+  <si>
+    <t>Giải thưởng trị giá 14 triệu đô sẽ thuộc về bất cứ ai bắt được đại sát thủ John Wick đã thúc đẩy John Wick và chú chó cưng lên đường chạy trốn.</t>
+  </si>
+  <si>
+    <t>Keanu Reeves, Halle Berry, Laurence Fishburne, Ian McShane</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_JohnWick3.mp4</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/08/16/11vhu9in_1920x1080-johnwick3-chuanbichientranh_296_168.webp</t>
+  </si>
+  <si>
+    <t>Toy story 2</t>
+  </si>
+  <si>
+    <t>​Câu Chuyện Đồ Chơi 2 tiếp tục cuộc phiêu lưu của Woody và Buzz Lightyear khi Andy (John Morris) tham dự trại hè và để mặc chúng ở nhà tự lo liệu.</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/14/b4skf5qr_1920x1080cauchuyendochoi2_296_168.webp</t>
+  </si>
+  <si>
+    <t>Trân Châu Cảng</t>
+  </si>
+  <si>
+    <t>Một sáng chủ nhật yên bình tháng 12 ở vùng đảo Hawaii bỗng nhiên tan vỡ, khi hạm đội bay của Đế quốc Nhật bất ngờ đột kích tiêu diệt hạm đội hải quân Mỹ tại căn cứ Trân Châu Cảng.</t>
+  </si>
+  <si>
+    <t>Ben Affleck, Josh Hartnett, Kate Beckinsale</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/28/f3oxedc9_1920x1080tranchaucang_296_168.webp</t>
+  </si>
+  <si>
+    <t>Vệ Binh Giải Ngân Hà</t>
+  </si>
+  <si>
+    <t>Phim nói về một phi công phản lực bị mắc kẹt trong không gian, và anh phải đoàn kết một nhóm người ngoài hành tinh để tạo thành một đội quân đủ khả năng đánh bại các mối đe dọa từ vũ trụ.</t>
+  </si>
+  <si>
+    <t>https://trailer.vieon.vn/Teaser_VeBinhDaiNganHa_chuanmoi.mp4</t>
+  </si>
+  <si>
+    <t>Chris Pratt, Zoe Saldana, Dave Bautista, Vin Diesel, Bradley Cooper</t>
+  </si>
+  <si>
+    <t>Phim tình cảm</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2021/12/28/odg8fgdq_1920x1080vebinhgiainganha_296_168.webp</t>
+  </si>
+  <si>
+    <t>Trò chơi sát thủ</t>
+  </si>
+  <si>
+    <t>Trò Chơi Sát Thủ là chuyện phim về hai sát thủ Vincent và Roland. Cả hai đều có cùng một mục tiêu cần phải khử, một người làm vì tiền và một người làm vì trả thù</t>
+  </si>
+  <si>
+    <t>Jean-Claude Van Damme, Scott Adkins, Kevin Chapman</t>
+  </si>
+  <si>
+    <t>https://static2.vieon.vn/vieplay-image/thumbnail_v4/2020/12/24/1m19h9dw_1920x1080trochoisatthu_296_168.webp</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/12-ky-binh-qua-cam.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/13-tieng.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/300.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/biet-doi-big-hero-6.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/biet-doi-sieu-anh-hung.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/annabell-ra-doi.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/chien-binh-mua-dong.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/toy-story-3.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/cuop-bien-vung-caribbean-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/da-quy.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/dai-chien-thanh-ansi.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/dai-chien-titan-live-1.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/dai-chien-titan-live-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/diep-vu-tam-giac-vang.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/gia-dinh-sieu-nhan.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/giai-cuu-nha-trang.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/harry-potter-1.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/harry-potter-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/khach-san-huyen-bi.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/ky-bang-ha-4.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/linh-ban-tia-my.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/long-an-co-mat.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/the-hobbit-3.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/spider-man-coming-home.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/transporter-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/nha-trang-that-thu-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/quy-quyet-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/john-wick-3.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/toy-story-2.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/tran-chau-cang.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/ve-binh-giai-ngan-ha.mp4</t>
+  </si>
+  <si>
+    <t>https://stream1.linhminaz.com/stream/1080/tro-choi-sat-thu.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +770,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -245,15 +817,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,115 +1145,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A96887D-E021-4561-8A6A-373B4871CD0C}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="177.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="166.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="74.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="166.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="106.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="81.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>2022</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
@@ -685,8 +1285,8 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>22</v>
@@ -698,27 +1298,27 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>2022</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
@@ -727,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>22</v>
@@ -739,27 +1339,27 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>2022</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -768,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>22</v>
@@ -780,27 +1380,27 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>2022</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
@@ -809,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>22</v>
@@ -821,27 +1421,27 @@
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>2022</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>21</v>
@@ -850,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>22</v>
@@ -862,27 +1462,27 @@
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>2022</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>21</v>
@@ -891,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>22</v>
@@ -903,27 +1503,27 @@
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>2022</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>21</v>
@@ -932,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>22</v>
@@ -944,27 +1544,27 @@
         <v>1</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>2022</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>21</v>
@@ -973,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>22</v>
@@ -985,27 +1585,27 @@
         <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>2022</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>21</v>
@@ -1014,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>22</v>
@@ -1026,93 +1626,1615 @@
         <v>1</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B12" s="1">
-        <v>2022</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>2018</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>32</v>
+      <c r="H12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>32</v>
+      <c r="M12" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>43</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>300</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="1">
+        <v>300</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="1">
+        <v>1</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2013</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="1">
+        <v>1</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="1">
+        <v>1</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="1">
+        <v>1</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{FEEBA0C1-77A6-4E43-972B-53D57F80BDAC}"/>
-    <hyperlink ref="Q3" r:id="rId2" display="https://stream1.linhminaz.com/stream/360/BOURNEMOUTH-BRENTFORD.mp4" xr:uid="{8D9912F7-F629-48DE-AFDC-BC37BFB17616}"/>
-    <hyperlink ref="Q4" r:id="rId3" display="https://stream1.linhminaz.com/stream/360/BRENTFORD - ARSENAL.mp4" xr:uid="{6A1CBC14-A06E-4E43-ADE3-3528C55BFEB6}"/>
-    <hyperlink ref="Q5" r:id="rId4" display="https://stream1.linhminaz.com/stream/360/EVERTON-WEST HAM.mp4" xr:uid="{517F98BD-C195-425E-A4A1-F1C53A1CA011}"/>
-    <hyperlink ref="Q6" r:id="rId5" display="https://stream1.linhminaz.com/stream/360/LEEDS UNITED-ASTON VILLA.mp4" xr:uid="{5F59AC3E-33F5-420A-81CF-4918680FAFA4}"/>
-    <hyperlink ref="Q7" r:id="rId6" display="https://stream1.linhminaz.com/stream/360/LEICESTER CITY-NOTTINGHAM FOREST.mp4" xr:uid="{8C06FFE1-352E-4160-8E6A-3E63E2EDFF77}"/>
-    <hyperlink ref="Q8" r:id="rId7" display="https://stream1.linhminaz.com/stream/360/LIVERPOOL-BRIGHTON.mp4" xr:uid="{A8B6E441-C8D5-4647-8611-66A5DCBB2D90}"/>
-    <hyperlink ref="Q9" r:id="rId8" display="https://stream1.linhminaz.com/stream/360/MAN CITY-MAN UNITED.mp4" xr:uid="{E84F9FC0-B2D8-44DB-94A4-B2194F597CC9}"/>
-    <hyperlink ref="Q10" r:id="rId9" display="https://stream1.linhminaz.com/stream/360/NEWCASTLE-BOURNEMOUTH.mp4" xr:uid="{E3E31409-9DA8-4536-B9E9-8769A313DE40}"/>
-    <hyperlink ref="Q11" r:id="rId10" display="https://stream1.linhminaz.com/stream/360/TOTTENHAM-LEICESTER CITY.mp4" xr:uid="{352DA551-DB11-442F-969F-205F74D2DC59}"/>
-    <hyperlink ref="Q12" r:id="rId11" display="https://stream1.linhminaz.com/stream/360/WEST HAM-WOLVES.mp4" xr:uid="{75671EF6-3F99-4B27-BE10-0664AB7C9E5B}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{FEEBA0C1-77A6-4E43-972B-53D57F80BDAC}"/>
+    <hyperlink ref="Q2" r:id="rId2" display="https://stream1.linhminaz.com/stream/360/BOURNEMOUTH-BRENTFORD.mp4" xr:uid="{8D9912F7-F629-48DE-AFDC-BC37BFB17616}"/>
+    <hyperlink ref="Q3" r:id="rId3" display="https://stream1.linhminaz.com/stream/360/BRENTFORD - ARSENAL.mp4" xr:uid="{6A1CBC14-A06E-4E43-ADE3-3528C55BFEB6}"/>
+    <hyperlink ref="Q4" r:id="rId4" display="https://stream1.linhminaz.com/stream/360/EVERTON-WEST HAM.mp4" xr:uid="{517F98BD-C195-425E-A4A1-F1C53A1CA011}"/>
+    <hyperlink ref="Q5" r:id="rId5" display="https://stream1.linhminaz.com/stream/360/LEEDS UNITED-ASTON VILLA.mp4" xr:uid="{5F59AC3E-33F5-420A-81CF-4918680FAFA4}"/>
+    <hyperlink ref="Q6" r:id="rId6" display="https://stream1.linhminaz.com/stream/360/LEICESTER CITY-NOTTINGHAM FOREST.mp4" xr:uid="{8C06FFE1-352E-4160-8E6A-3E63E2EDFF77}"/>
+    <hyperlink ref="Q7" r:id="rId7" display="https://stream1.linhminaz.com/stream/360/LIVERPOOL-BRIGHTON.mp4" xr:uid="{A8B6E441-C8D5-4647-8611-66A5DCBB2D90}"/>
+    <hyperlink ref="Q8" r:id="rId8" xr:uid="{E84F9FC0-B2D8-44DB-94A4-B2194F597CC9}"/>
+    <hyperlink ref="Q9" r:id="rId9" display="https://stream1.linhminaz.com/stream/360/NEWCASTLE-BOURNEMOUTH.mp4" xr:uid="{E3E31409-9DA8-4536-B9E9-8769A313DE40}"/>
+    <hyperlink ref="Q10" r:id="rId10" display="https://stream1.linhminaz.com/stream/360/TOTTENHAM-LEICESTER CITY.mp4" xr:uid="{352DA551-DB11-442F-969F-205F74D2DC59}"/>
+    <hyperlink ref="Q11" r:id="rId11" display="https://stream1.linhminaz.com/stream/360/WEST HAM-WOLVES.mp4" xr:uid="{75671EF6-3F99-4B27-BE10-0664AB7C9E5B}"/>
+    <hyperlink ref="H12" r:id="rId12" xr:uid="{73914679-8911-4B54-82EB-293C9BF4C557}"/>
+    <hyperlink ref="I12" r:id="rId13" xr:uid="{C1ECBF0E-6C58-4479-B3ED-294920269337}"/>
+    <hyperlink ref="M12" r:id="rId14" xr:uid="{95473C98-EE2A-4A7C-BA72-7687E973DC21}"/>
+    <hyperlink ref="Q12" r:id="rId15" display="https://stream1.linhminaz.com/stream/360/12-ky-binh-qua-cam.mp4" xr:uid="{41D4B9DC-CEA1-4179-B1DF-CAB57AA1DBF7}"/>
+    <hyperlink ref="M13" r:id="rId16" xr:uid="{05B13C88-EC29-4535-8C8E-DEFAA7515C1D}"/>
+    <hyperlink ref="H13" r:id="rId17" xr:uid="{6DF2EB56-614E-499A-A538-43A11A2AE228}"/>
+    <hyperlink ref="Q13" r:id="rId18" display="https://stream1.linhminaz.com/stream/360/13-tieng.mp4" xr:uid="{F4DC499C-0E26-42BD-B6ED-62E85C54A052}"/>
+    <hyperlink ref="M14" r:id="rId19" xr:uid="{4AD1E08C-D4C1-4098-8691-6AF457210538}"/>
+    <hyperlink ref="H14" r:id="rId20" xr:uid="{7A6D065C-66C5-43A1-B8DE-44767B4291E8}"/>
+    <hyperlink ref="Q14" r:id="rId21" display="https://stream1.linhminaz.com/stream/360/300.mp4" xr:uid="{7158E72A-4D81-4D3A-A65A-077F6B6AFED8}"/>
+    <hyperlink ref="I15" r:id="rId22" xr:uid="{3E1BDDD3-EA89-4F68-A93C-CFC7594EB771}"/>
+    <hyperlink ref="H15" r:id="rId23" xr:uid="{22736DA9-005F-4C10-9893-A2D8189AB2E4}"/>
+    <hyperlink ref="M15" r:id="rId24" xr:uid="{83ABFAD0-D8F3-4A49-AC4D-2A49E6BAA904}"/>
+    <hyperlink ref="Q15" r:id="rId25" display="https://stream1.linhminaz.com/stream/360/biet-doi-big-hero-6.mp4" xr:uid="{FF14CC0C-A254-4599-B60C-5B8F28291C26}"/>
+    <hyperlink ref="I16" r:id="rId26" xr:uid="{2117E5D3-CDA9-44D9-A64F-B5C7B730643C}"/>
+    <hyperlink ref="H16" r:id="rId27" xr:uid="{4DE8E8F7-3493-4B83-B51B-3E24352D634C}"/>
+    <hyperlink ref="M16" r:id="rId28" xr:uid="{596ABF88-0D4C-4096-ACD6-7A64D02AB022}"/>
+    <hyperlink ref="Q16" r:id="rId29" display="https://stream1.linhminaz.com/stream/360/biet-doi-sieu-anh-hung.mp4" xr:uid="{C9565C0C-8DAC-41E9-8E46-19F069A5F746}"/>
+    <hyperlink ref="I17" r:id="rId30" xr:uid="{8454A1F7-6CBC-40BB-815D-80E4E6215463}"/>
+    <hyperlink ref="H17" r:id="rId31" xr:uid="{7E7EBD85-0D88-42D3-A1F9-81E94C44C918}"/>
+    <hyperlink ref="M17" r:id="rId32" xr:uid="{E788F0F7-E15C-4AD4-AAF9-5595694B9F7D}"/>
+    <hyperlink ref="Q17" r:id="rId33" display="https://stream1.linhminaz.com/stream/360/annabell-ra-doi.mp4" xr:uid="{3924058C-6373-4595-9DB6-C153D0452614}"/>
+    <hyperlink ref="I18" r:id="rId34" xr:uid="{06E3C6F3-EC07-4391-A93C-38E44F37B2B8}"/>
+    <hyperlink ref="H18" r:id="rId35" xr:uid="{EB48102A-0FC0-43C1-9CF3-147D5F3D5CFD}"/>
+    <hyperlink ref="M18" r:id="rId36" xr:uid="{E38D3087-61C4-40EC-8272-A4A743BEAA07}"/>
+    <hyperlink ref="Q18" r:id="rId37" display="https://stream1.linhminaz.com/stream/360/chien-binh-mua-dong.mp4" xr:uid="{CD6C2AE9-6C46-4346-B996-B96983BAAEB8}"/>
+    <hyperlink ref="H19" r:id="rId38" xr:uid="{963739DB-ABC5-48FD-99C5-B47B92ECB7CA}"/>
+    <hyperlink ref="M19" r:id="rId39" xr:uid="{C9163C9B-A785-4154-AF7C-642768C43678}"/>
+    <hyperlink ref="Q19" r:id="rId40" display="https://stream1.linhminaz.com/stream/360/toy-story-3.mp4" xr:uid="{A106749E-192A-4302-B21A-EC4310955BDC}"/>
+    <hyperlink ref="H20" r:id="rId41" xr:uid="{C1726B4E-A4D6-473D-B931-611CD132A805}"/>
+    <hyperlink ref="M20" r:id="rId42" xr:uid="{E3676506-AD5F-450F-A57C-62C110897C10}"/>
+    <hyperlink ref="Q20" r:id="rId43" display="https://stream1.linhminaz.com/stream/360/cuop-bien-vung-caribbean-2.mp4" xr:uid="{26D1F439-DAD7-4AA6-B44D-2A07BBD61AE6}"/>
+    <hyperlink ref="I21" r:id="rId44" xr:uid="{EE5BC1FA-51DA-4983-AB7F-080B8C289D58}"/>
+    <hyperlink ref="H21" r:id="rId45" xr:uid="{02ADA3AA-B3AA-430C-95EA-AD665D3D76DB}"/>
+    <hyperlink ref="M21" r:id="rId46" xr:uid="{ED8181AC-B2AF-4D05-93A2-CB54FED3D0C1}"/>
+    <hyperlink ref="Q21" r:id="rId47" display="https://stream1.linhminaz.com/stream/360/da-quy.mp4" xr:uid="{7079A921-5067-48A3-B98E-C6412C1318DC}"/>
+    <hyperlink ref="H22" r:id="rId48" xr:uid="{BB01CE2A-FD7B-4FA7-BCFD-89B54C8D4F5E}"/>
+    <hyperlink ref="M22" r:id="rId49" xr:uid="{C4EFD814-FD7A-444A-B18C-946C338401F1}"/>
+    <hyperlink ref="Q22" r:id="rId50" display="https://stream1.linhminaz.com/stream/360/dai-chien-thanh-ansi.mp4" xr:uid="{0F4A0F8D-DB86-4671-BFCF-3AEC7DFCD1E6}"/>
+    <hyperlink ref="H23" r:id="rId51" xr:uid="{FF6E9929-562E-423E-9FF3-A6DBF72AE676}"/>
+    <hyperlink ref="M23" r:id="rId52" xr:uid="{AC14335B-3EEF-4DA1-907D-9CEA9F95C7BF}"/>
+    <hyperlink ref="Q23" r:id="rId53" display="https://stream1.linhminaz.com/stream/360/dai-chien-titan-live-1.mp4" xr:uid="{FECFA3EA-51DE-4FAC-A14A-C5574B6384FA}"/>
+    <hyperlink ref="H24" r:id="rId54" xr:uid="{4842753E-575F-45B8-8F64-71F8733EA428}"/>
+    <hyperlink ref="M24" r:id="rId55" xr:uid="{38DF3777-B832-476B-B917-66A8AA7A0806}"/>
+    <hyperlink ref="Q24" r:id="rId56" display="https://stream1.linhminaz.com/stream/360/dai-chien-titan-live-2.mp4" xr:uid="{D182A007-1B04-4D5D-A33C-F5C1D6C5EBB3}"/>
+    <hyperlink ref="M25" r:id="rId57" xr:uid="{59E9B982-D192-48CC-A982-7FC43878B2CB}"/>
+    <hyperlink ref="H25" r:id="rId58" xr:uid="{E6243614-CC25-48FA-B31C-DC9954CF13AA}"/>
+    <hyperlink ref="Q25" r:id="rId59" display="https://stream1.linhminaz.com/stream/360/diep-vu-tam-giac-vang.mp4" xr:uid="{363BDB49-CE5A-4C51-9412-F90B60408440}"/>
+    <hyperlink ref="I26" r:id="rId60" xr:uid="{674AAF42-64DA-48DF-A0B9-AD73C5614150}"/>
+    <hyperlink ref="H26" r:id="rId61" xr:uid="{2B2D3282-40DD-4FCE-B03E-2D3A3A9E82CD}"/>
+    <hyperlink ref="M26" r:id="rId62" xr:uid="{F9860143-435A-4D05-BE8D-38C49E2EE377}"/>
+    <hyperlink ref="Q26" r:id="rId63" display="https://stream1.linhminaz.com/stream/360/gia-dinh-sieu-nhan.mp4" xr:uid="{1FEE99B7-8CBC-4014-9FDD-24BA28655EBE}"/>
+    <hyperlink ref="I27" r:id="rId64" xr:uid="{DB9C2102-75E5-4E76-9016-3177F3CAA700}"/>
+    <hyperlink ref="H27" r:id="rId65" xr:uid="{554A3533-80E6-43E7-A328-D123FF7CAEF7}"/>
+    <hyperlink ref="M27" r:id="rId66" xr:uid="{707D7D36-F32A-4361-AE4E-DE4611C87C0D}"/>
+    <hyperlink ref="Q27" r:id="rId67" display="https://stream1.linhminaz.com/stream/360/giai-cuu-nha-trang.mp4" xr:uid="{22617B13-A0AB-4457-9EDF-D6D304EE97E8}"/>
+    <hyperlink ref="I28" r:id="rId68" xr:uid="{EA68BF31-8789-43D8-A0B4-CC0090059A08}"/>
+    <hyperlink ref="H28" r:id="rId69" xr:uid="{63AAE8B6-C940-4819-B795-E2EDD33F4548}"/>
+    <hyperlink ref="M28" r:id="rId70" xr:uid="{41314DC3-57BE-4189-9E86-ACDBBD546D1F}"/>
+    <hyperlink ref="Q28" r:id="rId71" display="https://stream1.linhminaz.com/stream/360/harry-potter-1.mp4" xr:uid="{C89963F8-3236-4FC4-85CE-20D782185A61}"/>
+    <hyperlink ref="I29" r:id="rId72" xr:uid="{F3A06449-5341-4B2F-9BC8-34D9FD78CBDC}"/>
+    <hyperlink ref="H29" r:id="rId73" xr:uid="{9AAF3298-E984-4E5A-8A22-57FE74DEA282}"/>
+    <hyperlink ref="M29" r:id="rId74" xr:uid="{C50B19CC-AE57-4339-B656-2F89609DC1FC}"/>
+    <hyperlink ref="Q29" r:id="rId75" display="https://stream1.linhminaz.com/stream/360/harry-potter-2.mp4" xr:uid="{5000C480-3F24-4D70-B2B3-BBA1F89B8FEA}"/>
+    <hyperlink ref="I30" r:id="rId76" xr:uid="{7A0B68C1-6206-4D42-8E59-95C0D744D776}"/>
+    <hyperlink ref="H30" r:id="rId77" xr:uid="{6E78685B-8BCA-409A-93B6-134BB6E523F9}"/>
+    <hyperlink ref="M30" r:id="rId78" xr:uid="{23156C10-9C3E-4F1F-B5F7-9188D627019A}"/>
+    <hyperlink ref="Q30" r:id="rId79" display="https://stream1.linhminaz.com/stream/360/khach-san-huyen-bi.mp4" xr:uid="{BC1F264C-3210-4ECB-A05E-6B1272CFAFBB}"/>
+    <hyperlink ref="H31" r:id="rId80" xr:uid="{5BB2FE88-B25C-45A6-BF44-7CB2324A51D0}"/>
+    <hyperlink ref="M31" r:id="rId81" xr:uid="{C52E63B6-526E-4730-ADEA-E1EB37AD48AB}"/>
+    <hyperlink ref="Q31" r:id="rId82" display="https://stream1.linhminaz.com/stream/360/ky-bang-ha-4.mp4" xr:uid="{6E447BF8-B043-4FD9-B5F5-0CDB424A9453}"/>
+    <hyperlink ref="I32" r:id="rId83" xr:uid="{8E318652-3658-49DF-BBC8-1BC965093AEA}"/>
+    <hyperlink ref="M32" r:id="rId84" xr:uid="{3A8E8329-BEC8-4BD7-A188-4FD2B64AF9B3}"/>
+    <hyperlink ref="H32" r:id="rId85" xr:uid="{9237B433-92A2-409A-8853-12453C02137F}"/>
+    <hyperlink ref="Q32" r:id="rId86" display="https://stream1.linhminaz.com/stream/360/linh-ban-tia-my.mp4" xr:uid="{69250D0D-FB5E-4830-A4F9-0D7C4488A72A}"/>
+    <hyperlink ref="H33" r:id="rId87" xr:uid="{FF3D95DD-FD05-4465-AF40-9AEA9216443A}"/>
+    <hyperlink ref="M33" r:id="rId88" xr:uid="{ACB60DF4-4C34-4BAE-B67E-2E9C7AF3F77C}"/>
+    <hyperlink ref="Q33" r:id="rId89" display="https://stream1.linhminaz.com/stream/360/long-an-co-mat.mp4" xr:uid="{BA6E00A0-68D5-48E8-B944-5F7730440F99}"/>
+    <hyperlink ref="I34" r:id="rId90" xr:uid="{87338767-1FFE-429A-8C42-23BA4DE85DF6}"/>
+    <hyperlink ref="H34" r:id="rId91" xr:uid="{73EDBBCB-9142-4ACF-BC8C-495C7C0CB975}"/>
+    <hyperlink ref="M34" r:id="rId92" xr:uid="{A4243189-B4A6-4C4D-B886-328E404F1159}"/>
+    <hyperlink ref="Q34" r:id="rId93" display="https://stream1.linhminaz.com/stream/360/the-hobbit-3.mp4" xr:uid="{B5459D53-CC50-4544-AE22-27D61401E546}"/>
+    <hyperlink ref="I35" r:id="rId94" xr:uid="{B1146278-4963-469C-9217-99D514BF153B}"/>
+    <hyperlink ref="H35" r:id="rId95" xr:uid="{812EA7E5-8F0F-4A76-90C4-7998E9DC7149}"/>
+    <hyperlink ref="M35" r:id="rId96" xr:uid="{E8B9CA35-8535-4AA2-8DB1-73A5684B9EDF}"/>
+    <hyperlink ref="Q35" r:id="rId97" xr:uid="{9CF4D1B7-3520-4D9A-BC63-06D348007D85}"/>
+    <hyperlink ref="H36" r:id="rId98" xr:uid="{48C94E24-E3F7-48D7-8FCD-E3CA15A55AEB}"/>
+    <hyperlink ref="M36" r:id="rId99" xr:uid="{A3860DE7-7910-4F07-AE88-5A6AC09A1B39}"/>
+    <hyperlink ref="Q36" r:id="rId100" display="https://stream1.linhminaz.com/stream/360/transporter-2.mp4" xr:uid="{91249DC2-87A6-46E9-8C7E-8A8DC7511A9E}"/>
+    <hyperlink ref="I37" r:id="rId101" xr:uid="{6EC9A4C2-01E9-495E-837B-9CA94E6C6956}"/>
+    <hyperlink ref="H37" r:id="rId102" xr:uid="{11A9248D-4144-4B12-B0CB-686691B979A5}"/>
+    <hyperlink ref="M37" r:id="rId103" xr:uid="{89F8DCFD-5EA3-43C8-9EE2-AAE16F652A37}"/>
+    <hyperlink ref="Q37" r:id="rId104" display="https://stream1.linhminaz.com/stream/360/nha-trang-that-thu-2.mp4" xr:uid="{856DD5D5-E479-4158-90B8-E617AB13F387}"/>
+    <hyperlink ref="I38" r:id="rId105" xr:uid="{C87A2BBB-80BA-4AAC-B46B-3E19A9EE715F}"/>
+    <hyperlink ref="H38" r:id="rId106" xr:uid="{7E020FA4-0DEE-44F1-AC53-44068C2EC350}"/>
+    <hyperlink ref="M38" r:id="rId107" xr:uid="{3690AB15-3B90-4609-BCC0-F3032EA5758B}"/>
+    <hyperlink ref="Q38" r:id="rId108" display="https://stream1.linhminaz.com/stream/360/quy-quyet-2.mp4" xr:uid="{256A1335-79E9-4EBF-9B09-0F265DC1CF02}"/>
+    <hyperlink ref="I39" r:id="rId109" xr:uid="{44E1C93C-5AC3-4027-BB12-3C9EF197307A}"/>
+    <hyperlink ref="H39" r:id="rId110" xr:uid="{0ED9F0DB-9134-4726-9642-74919C586412}"/>
+    <hyperlink ref="M39" r:id="rId111" xr:uid="{FFFE5F31-BADE-45ED-9506-01164A8BC9E9}"/>
+    <hyperlink ref="Q39" r:id="rId112" display="https://stream1.linhminaz.com/stream/360/john-wick-3.mp4" xr:uid="{C0473F0E-AC2F-4D64-8598-961F04BC372C}"/>
+    <hyperlink ref="H40" r:id="rId113" xr:uid="{74BC58D1-93F3-4DCA-B53E-64FF3CCFB63B}"/>
+    <hyperlink ref="M40" r:id="rId114" xr:uid="{67CEF036-E9D0-40C3-8819-F9073EAAE428}"/>
+    <hyperlink ref="Q40" r:id="rId115" display="https://stream1.linhminaz.com/stream/360/toy-story-2.mp4" xr:uid="{D494E7FA-DC1E-488E-AB28-4736176C1030}"/>
+    <hyperlink ref="H41" r:id="rId116" xr:uid="{6E16D209-8927-4BD0-B864-E933B896E66B}"/>
+    <hyperlink ref="M41" r:id="rId117" xr:uid="{01C3F3C0-C8FD-41B2-A718-C120F563013C}"/>
+    <hyperlink ref="Q41" r:id="rId118" display="https://stream1.linhminaz.com/stream/360/tran-chau-cang.mp4" xr:uid="{EC1775D9-FC4A-4477-9DC9-904F72D99CE2}"/>
+    <hyperlink ref="I42" r:id="rId119" xr:uid="{CE65F7F8-F106-4972-BD0B-BF10810DDAA0}"/>
+    <hyperlink ref="H42" r:id="rId120" xr:uid="{F66B311F-D7DB-42E0-B057-9CD8D56DFB6D}"/>
+    <hyperlink ref="M42" r:id="rId121" xr:uid="{FCC2F4D4-79CB-4AE7-9220-D12ECB305E95}"/>
+    <hyperlink ref="Q42" r:id="rId122" display="https://stream1.linhminaz.com/stream/360/ve-binh-giai-ngan-ha.mp4" xr:uid="{2CE2FEA9-4523-4073-A9A6-E01EC783418C}"/>
+    <hyperlink ref="H43" r:id="rId123" xr:uid="{865D0386-0A67-40B0-8CBE-106854616BD7}"/>
+    <hyperlink ref="M43" r:id="rId124" xr:uid="{D1892CC6-A5E8-4AF0-A99F-4F4AD3F6EF04}"/>
+    <hyperlink ref="Q43" r:id="rId125" display="https://stream1.linhminaz.com/stream/360/tro-choi-sat-thu.mp4" xr:uid="{8481B0CF-B18A-4584-A278-FDF5F575F78F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId126"/>
 </worksheet>
 </file>
</xml_diff>